<commit_message>
non-preemptive priority queue simulation and exact analysis
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsjnancy/Desktop/Research/simulation_tmle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A3F727-FB34-DF42-AD3B-2DEBD2FDCFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202D104E-6BED-AF45-99DE-9737A821CF55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4400" yWindow="460" windowWidth="23000" windowHeight="16120" activeTab="1" xr2:uid="{425F17CA-4810-A644-B01D-BD0370C78A9D}"/>
+    <workbookView xWindow="6620" yWindow="460" windowWidth="21760" windowHeight="16120" activeTab="1" xr2:uid="{425F17CA-4810-A644-B01D-BD0370C78A9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
   <si>
     <t>Backlog</t>
   </si>
@@ -45,16 +45,7 @@
     <t>Wait time tracker</t>
   </si>
   <si>
-    <t>90th percentile for number in system &amp; number in queue</t>
-  </si>
-  <si>
-    <t>G/G/1 with appointments</t>
-  </si>
-  <si>
     <t>M(t)/G(t, n)/∞</t>
-  </si>
-  <si>
-    <t>M/G/1 exact analysis</t>
   </si>
   <si>
     <t>a_i' = d_i + p_i (deterministic + noise)</t>
@@ -177,19 +168,7 @@
     <t>No merging to master branch required</t>
   </si>
   <si>
-    <t>M/G/1 priority queue</t>
-  </si>
-  <si>
     <t>Arrivals of next customer is independent of the punctuality of the previous customer</t>
-  </si>
-  <si>
-    <t>created a new Python class</t>
-  </si>
-  <si>
-    <t>Plotting performance measures for individual classes in multi-class M/G/1 queues</t>
-  </si>
-  <si>
-    <t>added code in plotting.py</t>
   </si>
   <si>
     <t xml:space="preserve">1. This assumes that customer already in service cannot be interrupted when a customer with a higher priority arrives. 
@@ -301,23 +280,180 @@
     <t>Completed (August 9, 2020)</t>
   </si>
   <si>
-    <t>add exact analysis graphs to the performance measures plots</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Exact analysis for the expected values uses the Pollaczek-Khinchin mean formulas directly.
 2. Exact analysis for the 90th percentile values uses the PK transform formulas. The CDF for the empirical distribution is obtained by inverting the Laplace transform formula. Trial and error is used to obtain the 90th percentile values. Time points are tried starting from 1e-08 with 0.25 increments until the CDF is &gt;= 0.9 </t>
   </si>
   <si>
-    <t>SIMULATION
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SIMULATION (FCFS &amp; Non-preemptive Priority)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 1. Plotting expected values and 90th percentiles with 95% CI (confidence level adjustable)
 2. For k=1 class, fixed λ=1, μ=1.1, μ'= [2, 2.5, 3], P(intervention)=[0, 0.1, …, 1.0] --&gt; To simulate for k classes, additional variables can be added if required.
 3. Four performance measures: TIS, WIQ, NIS, NIQ
 4. Supports generating plots for all classes as well as for individual classes
-EXACT ANALYSIS
-1. Plotting expected values and 90th percentiles for 4 performance measures (TIS, WIQ, NIS, NIQ)</t>
-  </si>
-  <si>
-    <t>2020-08-09 (Nancy)</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EXACT ANALYSIS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Single Class FCFS:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Expected Values and 90th Percentiles (TIS, WIQ, NIS, NIQ)
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Non-preemptive Priority (Two Classes):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Expected Values (TIS, WIQ, NIS, NIQ)</t>
+    </r>
+  </si>
+  <si>
+    <t>2020-08-17 (Nancy)</t>
+  </si>
+  <si>
+    <t>plotting_all_results.py</t>
+  </si>
+  <si>
+    <t>1. Compare results from 4 methods on single plot (simulation, exact analysis, parametric, non-parametric) --&gt; TIS, WIQ --&gt; single class FCFS</t>
+  </si>
+  <si>
+    <t>2020-08-14
+(Nancy)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Generate simulation and exact analysis plots for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Non-preemptive Priority Queues (Two Classes)</t>
+    </r>
+  </si>
+  <si>
+    <t>Modified plotting.py</t>
+  </si>
+  <si>
+    <t>Created a new Python class</t>
+  </si>
+  <si>
+    <t>M/G/1 Non-preemptive Priority Queue</t>
+  </si>
+  <si>
+    <t>G/G/1 with appointments
+First Come, First Served (FCFS)</t>
+  </si>
+  <si>
+    <t>Computing 90th percentile for number in system &amp; number in queue</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plotting performance measures for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>individual classes in Multi-class M/G/1 Queues</t>
+    </r>
+  </si>
+  <si>
+    <t>M/G/1 Exact Analysis</t>
+  </si>
+  <si>
+    <t>Added exact analysis graphs to the performance measures plots
+Modified plotting.py</t>
+  </si>
+  <si>
+    <t>Completed (August 17, 2020)</t>
+  </si>
+  <si>
+    <t>1. Exact analysis --&gt; hyperexponential distribution, mean formulas from lecture notes
+2. Simulation --&gt; same calculation methods as FCFS
+3. Plots --&gt; all classes, class 1, class 2</t>
+  </si>
+  <si>
+    <t>1. Supports plotting for all classes and individual classes</t>
   </si>
 </sst>
 </file>
@@ -844,18 +980,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C94F3266-32D3-C749-ADFF-5F3E2FC86E34}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="109" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A8" zoomScale="109" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="9.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16" style="5" customWidth="1"/>
     <col min="5" max="5" width="49" style="9" customWidth="1"/>
     <col min="6" max="6" width="6.1640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -864,7 +1000,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -873,10 +1009,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="34">
@@ -888,11 +1024,11 @@
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="20" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E2" s="9"/>
       <c r="G2" s="22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="34">
@@ -900,70 +1036,70 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="20" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E3" s="9"/>
       <c r="G3" s="23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="42" customHeight="1">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="24" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="69" thickBot="1">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>14</v>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>44</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>51</v>
       </c>
       <c r="E5" s="9"/>
       <c r="G5" s="25" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="102">
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>38</v>
+      <c r="B6" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G6" s="19"/>
     </row>
@@ -972,48 +1108,67 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="G7" s="19"/>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="68">
+    <row r="8" spans="1:7" ht="136">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>5</v>
+      <c r="B8" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="136">
+        <v>61</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="68">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>55</v>
-      </c>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="68">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1022,17 +1177,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C969E3-5586-DF43-842E-32538FE64F98}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.1640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" style="8" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="8" bestFit="1" customWidth="1"/>
@@ -1043,22 +1198,22 @@
   <sheetData>
     <row r="1" spans="1:8" ht="35" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="51">
@@ -1066,19 +1221,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="52" thickBot="1">
@@ -1086,126 +1241,147 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="221">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="255">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="205" thickBot="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="69" thickBot="1">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="119">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="204">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="18"/>
-    </row>
-    <row r="7" spans="1:8" ht="34">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="119">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="68">
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8" ht="34">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="D8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="68">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>35</v>
+      <c r="F9" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>